<commit_message>
Week 3 ICM Tracker
</commit_message>
<xml_diff>
--- a/docs/ICM_Tracker.xlsx
+++ b/docs/ICM_Tracker.xlsx
@@ -25,34 +25,34 @@
     <t>Chris</t>
   </si>
   <si>
-    <t>Week 1</t>
-  </si>
-  <si>
-    <t>Week 2</t>
-  </si>
-  <si>
-    <t>Week 3</t>
-  </si>
-  <si>
-    <t>Week 4</t>
-  </si>
-  <si>
-    <t>Week 5</t>
-  </si>
-  <si>
-    <t>Week 6</t>
-  </si>
-  <si>
-    <t>Week 7</t>
-  </si>
-  <si>
-    <t>Week 8</t>
-  </si>
-  <si>
-    <t>Week 9</t>
-  </si>
-  <si>
-    <t>Week 10</t>
+    <t>Week 1: 10th Oct</t>
+  </si>
+  <si>
+    <t>Week 2: 17th Oct</t>
+  </si>
+  <si>
+    <t>Week 3: 24th Oct</t>
+  </si>
+  <si>
+    <t>Week 4: 31st Oct</t>
+  </si>
+  <si>
+    <t>Week 5: 7th Nov</t>
+  </si>
+  <si>
+    <t>Week 6: 14th Nov</t>
+  </si>
+  <si>
+    <t>Week 7: 21st Nov</t>
+  </si>
+  <si>
+    <t>Week 8: 28th Nov</t>
+  </si>
+  <si>
+    <t>Week 9: 5th Dec</t>
+  </si>
+  <si>
+    <t>Week 10: 12th Dec</t>
   </si>
   <si>
     <t>Total</t>
@@ -149,6 +149,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="17.57"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="B1" s="1" t="s">
@@ -202,6 +205,18 @@
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="B4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
@@ -244,19 +259,19 @@
       </c>
       <c r="B13" s="5">
         <f t="shared" ref="B13:E13" si="1">SUM(B2:B11)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13" s="5">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D13" s="5">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
@@ -286,7 +301,7 @@
       </c>
       <c r="B16" s="5">
         <f>SUM(B13:E13)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>